<commit_message>
finished Impending Date Reduction! Still much to do, but good for alpha
</commit_message>
<xml_diff>
--- a/Calibration_TMA_SOP Schedule_Master Form 101359.xlsx
+++ b/Calibration_TMA_SOP Schedule_Master Form 101359.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="24840" windowHeight="12720" tabRatio="912" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="24840" windowHeight="12720" tabRatio="912" firstSheet="7" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Items for multiple tests" sheetId="4" r:id="rId1"/>
@@ -26473,13 +26473,13 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26687,6 +26687,14 @@
       <c r="G9">
         <v>7</v>
       </c>
+    </row>
+    <row r="10" spans="1:10" s="141" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="73"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -31525,7 +31533,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" ht="63" hidden="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -31630,7 +31638,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="42" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" ht="63" x14ac:dyDescent="0.4">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -31717,7 +31725,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="42" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" ht="63" x14ac:dyDescent="0.4">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -31851,7 +31859,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="63" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" ht="84" x14ac:dyDescent="0.4">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -32316,7 +32324,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="63" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" ht="84" x14ac:dyDescent="0.4">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -34784,7 +34792,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -34815,7 +34823,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -34896,7 +34904,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -34925,7 +34933,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -50937,7 +50945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="63" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" ht="84" x14ac:dyDescent="0.4">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
         <v>1330</v>
@@ -52451,7 +52459,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="84" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:15" ht="105" x14ac:dyDescent="0.4">
       <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
         <v>1411</v>
@@ -52698,7 +52706,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="63" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" ht="84" x14ac:dyDescent="0.4">
       <c r="A79" s="2"/>
       <c r="B79" s="2" t="s">
         <v>1453</v>
@@ -55433,7 +55441,7 @@
   </sheetPr>
   <dimension ref="A1:P265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I2" sqref="I1:I1048576"/>
       <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>

</xml_diff>

<commit_message>
fixed a weird copy-paste bug
</commit_message>
<xml_diff>
--- a/Calibration_TMA_SOP Schedule_Master Form 101359.xlsx
+++ b/Calibration_TMA_SOP Schedule_Master Form 101359.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="24840" windowHeight="12720" tabRatio="912" firstSheet="7" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="24840" windowHeight="12720" tabRatio="912" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Items for multiple tests" sheetId="4" r:id="rId1"/>
@@ -26475,7 +26475,7 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -31533,7 +31533,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" ht="63" hidden="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -31638,7 +31638,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="42" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" ht="63" x14ac:dyDescent="0.4">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -31725,7 +31725,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="42" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" ht="63" x14ac:dyDescent="0.4">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -31859,7 +31859,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="63" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" ht="84" x14ac:dyDescent="0.4">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -32324,7 +32324,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="63" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" ht="84" x14ac:dyDescent="0.4">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -34792,7 +34792,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -34823,7 +34823,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -34904,7 +34904,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -34933,7 +34933,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -49095,9 +49095,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52459,7 +52459,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="84" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:15" ht="105" x14ac:dyDescent="0.4">
       <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
         <v>1411</v>
@@ -52648,7 +52648,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="63" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:15" ht="84" x14ac:dyDescent="0.4">
       <c r="A77" s="2"/>
       <c r="B77" s="4" t="s">
         <v>1407</v>
@@ -52706,7 +52706,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="63" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" ht="84" x14ac:dyDescent="0.4">
       <c r="A79" s="2"/>
       <c r="B79" s="2" t="s">
         <v>1453</v>

</xml_diff>